<commit_message>
Added photos and updated db scripts
</commit_message>
<xml_diff>
--- a/dinghies.xlsx
+++ b/dinghies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soarsi\workspace\github\dinghy-search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53373745-EFC4-4356-AE83-056D4679C366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF5B810-451E-41D2-9F97-0942D02DA5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="22530" windowHeight="15585" xr2:uid="{424A2331-99F2-4D2E-BF59-9192B1CDA9D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{424A2331-99F2-4D2E-BF59-9192B1CDA9D6}"/>
   </bookViews>
   <sheets>
     <sheet name="RS" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="248">
   <si>
     <t>name</t>
   </si>
@@ -426,9 +426,6 @@
     <t>/images/logos/international-505-logo.png</t>
   </si>
   <si>
-    <t>/images/470-dinghy.jpg</t>
-  </si>
-  <si>
     <t>/images/tera-pro.jpg</t>
   </si>
   <si>
@@ -496,6 +493,297 @@
   </si>
   <si>
     <t>/images/logos/RSVision.jpg</t>
+  </si>
+  <si>
+    <t>/images/aero-5.jpg</t>
+  </si>
+  <si>
+    <t>/images/aero-6.jpg</t>
+  </si>
+  <si>
+    <t>/images/aero-7.jpg</t>
+  </si>
+  <si>
+    <t>/images/aero-9.jpg</t>
+  </si>
+  <si>
+    <t>/images/2000.jpg</t>
+  </si>
+  <si>
+    <t>/images/rsfeva.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs-quest.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs-toura.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs-vareo.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs-venture.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs-vision.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs-zest.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs-neo.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs100.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs200.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs300.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs400.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs500.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs600.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs700.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs800.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs-cat14.jpg</t>
+  </si>
+  <si>
+    <t>/images/rs-cat16.jpg</t>
+  </si>
+  <si>
+    <t>/images/ILCA4.jpg</t>
+  </si>
+  <si>
+    <t>/images/ILCA6.jpg</t>
+  </si>
+  <si>
+    <t>/images/ILCA7.jpg</t>
+  </si>
+  <si>
+    <t>/images/blaze.jpg</t>
+  </si>
+  <si>
+    <t>/images/contender.jpg</t>
+  </si>
+  <si>
+    <t>/images/europe.jpg</t>
+  </si>
+  <si>
+    <t>/images/finn.jpg</t>
+  </si>
+  <si>
+    <t>/images/fusion.jpg</t>
+  </si>
+  <si>
+    <t>/images/k1.jpg</t>
+  </si>
+  <si>
+    <t>/images/ok.jpg</t>
+  </si>
+  <si>
+    <t>/images/optimist.jpg</t>
+  </si>
+  <si>
+    <t>/images/phantom.jpg</t>
+  </si>
+  <si>
+    <t>/images/solo.jpg</t>
+  </si>
+  <si>
+    <t>/images/solution.jpg</t>
+  </si>
+  <si>
+    <t>/images/streaker.jpg</t>
+  </si>
+  <si>
+    <t>/images/supernova.jpg</t>
+  </si>
+  <si>
+    <t>/images/byte-cII.jpg</t>
+  </si>
+  <si>
+    <t>/images/international-canoe.jpg</t>
+  </si>
+  <si>
+    <t>/images/international-moth.jpg</t>
+  </si>
+  <si>
+    <t>/images/musto-skiff.jpg</t>
+  </si>
+  <si>
+    <t>/images/topper.jpg</t>
+  </si>
+  <si>
+    <t>/images/waszp.jpg</t>
+  </si>
+  <si>
+    <t>/images/devoti-d-one.jpg</t>
+  </si>
+  <si>
+    <t>/images/devoti-d-zero.jpg</t>
+  </si>
+  <si>
+    <t>/images/hadron-h2.jpg</t>
+  </si>
+  <si>
+    <t>/images/lightning-368.jpg</t>
+  </si>
+  <si>
+    <t>/images/420.jpg</t>
+  </si>
+  <si>
+    <t>/images/505.jpg</t>
+  </si>
+  <si>
+    <t>/images/470.jpg</t>
+  </si>
+  <si>
+    <t>/images/29er.jpg</t>
+  </si>
+  <si>
+    <t>/images/49er.jpg</t>
+  </si>
+  <si>
+    <t>/images/49er-fx.jpg</t>
+  </si>
+  <si>
+    <t>/images/b14.jpg</t>
+  </si>
+  <si>
+    <t>/images/albacore.jpg</t>
+  </si>
+  <si>
+    <t>Comet</t>
+  </si>
+  <si>
+    <t>/images/comet.jpg</t>
+  </si>
+  <si>
+    <t>/images/buzz.jpg</t>
+  </si>
+  <si>
+    <t>/images/cadet.jpg</t>
+  </si>
+  <si>
+    <t>/images/cherub.jpg</t>
+  </si>
+  <si>
+    <t>/images/comet-trio.jpg</t>
+  </si>
+  <si>
+    <t>/images/enterprise.jpg</t>
+  </si>
+  <si>
+    <t>/images/fireball.jpg</t>
+  </si>
+  <si>
+    <t>/images/flying-fifteen.jpg</t>
+  </si>
+  <si>
+    <t>/images/gp14.jpg</t>
+  </si>
+  <si>
+    <t>/images/firefly.jpg</t>
+  </si>
+  <si>
+    <t>/images/graduate.jpg</t>
+  </si>
+  <si>
+    <t>/images/hornet.jpg</t>
+  </si>
+  <si>
+    <t>/images/international-14.jpg</t>
+  </si>
+  <si>
+    <t>/images/kestrel.jpg</t>
+  </si>
+  <si>
+    <t>/images/lark.jpg</t>
+  </si>
+  <si>
+    <t>/images/merlin-rocket.jpg</t>
+  </si>
+  <si>
+    <t>/images/miracle.jpg</t>
+  </si>
+  <si>
+    <t>/images/mirror.jpg</t>
+  </si>
+  <si>
+    <t>/images/national-12.jpg</t>
+  </si>
+  <si>
+    <t>/images/osprey.jpg</t>
+  </si>
+  <si>
+    <t>/images/seafly.jpg</t>
+  </si>
+  <si>
+    <t>/images/scorpion.jpg</t>
+  </si>
+  <si>
+    <t>/images/tasar.jpg</t>
+  </si>
+  <si>
+    <t>/images/wanderer.jpg</t>
+  </si>
+  <si>
+    <t>/images/wayfarer.jpg</t>
+  </si>
+  <si>
+    <t>/images/k6.jpg</t>
+  </si>
+  <si>
+    <t>/images/alto.jpg</t>
+  </si>
+  <si>
+    <t>/images/challenger.jpg</t>
+  </si>
+  <si>
+    <t>/images/spitfire.jpg</t>
+  </si>
+  <si>
+    <t>/images/dart-15.jpg</t>
+  </si>
+  <si>
+    <t>/images/dart-18.jpg</t>
+  </si>
+  <si>
+    <t>/images/hurricane.jpg</t>
+  </si>
+  <si>
+    <t>/images/nacra-15.jpg</t>
+  </si>
+  <si>
+    <t>/images/nacra-17.jpg</t>
+  </si>
+  <si>
+    <t>/images/nacra-500.jpg</t>
+  </si>
+  <si>
+    <t>/images/nacra-570.jpg</t>
+  </si>
+  <si>
+    <t>/images/nacra-f16.jpg</t>
+  </si>
+  <si>
+    <t>/images/nacra-f18.jpg</t>
+  </si>
+  <si>
+    <t>/images/nacra-f20.jpg</t>
   </si>
 </sst>
 </file>
@@ -885,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170DDF5A-0F38-402E-9EB4-88FDC06AA77D}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,16 +1182,16 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="6" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="5" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -997,7 +1285,10 @@
         <v>10.119999999999999</v>
       </c>
       <c r="O2" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="P2" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1041,7 +1332,10 @@
         <v>5.2</v>
       </c>
       <c r="O3" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="P3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1085,7 +1379,10 @@
         <v>6.3</v>
       </c>
       <c r="O4" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="P4" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1129,7 +1426,10 @@
         <v>7.4</v>
       </c>
       <c r="O5" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="P5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1173,7 +1473,10 @@
         <v>8.9</v>
       </c>
       <c r="O6" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="P6" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1217,7 +1520,10 @@
         <v>9</v>
       </c>
       <c r="O7" t="s">
-        <v>139</v>
+        <v>138</v>
+      </c>
+      <c r="P7" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1261,7 +1567,10 @@
         <v>12.82</v>
       </c>
       <c r="O8" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="P8" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1308,7 +1617,10 @@
         <v>7</v>
       </c>
       <c r="O9" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="P9" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1349,7 +1661,10 @@
         <v>6</v>
       </c>
       <c r="O10" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+      <c r="P10" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1393,7 +1708,10 @@
         <v>11</v>
       </c>
       <c r="O11" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="P11" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1437,10 +1755,10 @@
         <v>4.8</v>
       </c>
       <c r="O12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1484,10 +1802,10 @@
         <v>3.7</v>
       </c>
       <c r="O13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1531,7 +1849,10 @@
         <v>14.6</v>
       </c>
       <c r="O14" t="s">
-        <v>145</v>
+        <v>144</v>
+      </c>
+      <c r="P14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1578,7 +1899,10 @@
         <v>9.9</v>
       </c>
       <c r="O15" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="P15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1622,10 +1946,13 @@
         <v>14</v>
       </c>
       <c r="O16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="P16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1669,10 +1996,13 @@
         <v>12</v>
       </c>
       <c r="O17" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="P17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1710,10 +2040,13 @@
         <v>7.1</v>
       </c>
       <c r="O18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="P18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1754,10 +2087,13 @@
         <v>12.5</v>
       </c>
       <c r="O19" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="P19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1801,10 +2137,13 @@
         <v>12.5</v>
       </c>
       <c r="O20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="P20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1848,10 +2187,13 @@
         <v>8.2899999999999991</v>
       </c>
       <c r="O21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="P21" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1892,10 +2234,13 @@
         <v>10</v>
       </c>
       <c r="O22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="P22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1939,10 +2284,13 @@
         <v>13.94</v>
       </c>
       <c r="O23" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="P23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1986,10 +2334,13 @@
         <v>14</v>
       </c>
       <c r="O24" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="P24" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2030,10 +2381,13 @@
         <v>12.14</v>
       </c>
       <c r="O25" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="P25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2077,10 +2431,13 @@
         <v>16</v>
       </c>
       <c r="O26" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="P26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2124,7 +2481,10 @@
         <v>21</v>
       </c>
       <c r="O27" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="P27" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2141,7 +2501,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,6 +2510,7 @@
     <col min="10" max="11" width="9.140625" style="3"/>
     <col min="13" max="13" width="9.140625" style="5"/>
     <col min="15" max="15" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2245,6 +2606,9 @@
       <c r="O2" t="s">
         <v>124</v>
       </c>
+      <c r="P2" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2289,6 +2653,9 @@
       <c r="O3" t="s">
         <v>124</v>
       </c>
+      <c r="P3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2332,6 +2699,9 @@
       </c>
       <c r="O4" t="s">
         <v>124</v>
+      </c>
+      <c r="P4" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2342,10 +2712,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58FFF61-D2B4-441A-BA1C-302767283A2C}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,14 +2723,15 @@
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="3"/>
     <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="5"/>
     <col min="14" max="14" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2453,6 +2824,9 @@
       <c r="M2" s="5">
         <v>10.4</v>
       </c>
+      <c r="P2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2494,16 +2868,16 @@
       <c r="M3" s="5">
         <v>6.8</v>
       </c>
+      <c r="P3" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="C4">
-        <v>966</v>
+        <v>1210</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2521,30 +2895,33 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>4.88</v>
+        <v>3.45</v>
       </c>
       <c r="K4" s="3">
-        <v>1.5</v>
+        <v>1.37</v>
       </c>
       <c r="L4">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="M4" s="5">
-        <v>10.3</v>
+        <v>6.5</v>
+      </c>
+      <c r="P4" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="C5">
-        <v>950</v>
+        <v>966</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2559,36 +2936,36 @@
         <v>0</v>
       </c>
       <c r="H5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="3">
-        <v>4.2300000000000004</v>
+        <v>4.88</v>
       </c>
       <c r="K5" s="3">
-        <v>2.31</v>
+        <v>1.5</v>
       </c>
       <c r="L5">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="M5" s="5">
-        <v>11.5</v>
-      </c>
-      <c r="N5" s="5">
-        <v>13.2</v>
+        <v>10.3</v>
+      </c>
+      <c r="P5" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
       </c>
       <c r="C6">
-        <v>1032</v>
+        <v>950</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2603,30 +2980,39 @@
         <v>0</v>
       </c>
       <c r="H6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" s="3">
-        <v>4.2</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="K6" s="3">
-        <v>1.42</v>
+        <v>2.31</v>
       </c>
       <c r="L6">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="M6" s="5">
-        <v>8.1</v>
+        <v>11.5</v>
+      </c>
+      <c r="N6" s="5">
+        <v>13.2</v>
+      </c>
+      <c r="P6" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
       </c>
       <c r="C7">
-        <v>1147</v>
+        <v>1032</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2647,27 +3033,27 @@
         <v>0</v>
       </c>
       <c r="J7" s="3">
-        <v>3.35</v>
+        <v>4.2</v>
       </c>
       <c r="K7" s="3">
-        <v>1.38</v>
+        <v>1.42</v>
       </c>
       <c r="L7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M7" s="5">
-        <v>7</v>
+        <v>8.1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8">
-        <v>1047</v>
+        <v>1147</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2688,27 +3074,30 @@
         <v>0</v>
       </c>
       <c r="J8" s="3">
-        <v>4.53</v>
+        <v>3.35</v>
       </c>
       <c r="K8" s="3">
-        <v>1.58</v>
+        <v>1.38</v>
       </c>
       <c r="L8">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="M8" s="5">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="P8" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>52</v>
       </c>
       <c r="C9">
-        <v>1280</v>
+        <v>1047</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2729,27 +3118,30 @@
         <v>0</v>
       </c>
       <c r="J9" s="3">
-        <v>3.6</v>
+        <v>4.53</v>
       </c>
       <c r="K9" s="3">
-        <v>1.45</v>
+        <v>1.58</v>
       </c>
       <c r="L9">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="M9" s="5">
-        <v>6.45</v>
+        <v>10</v>
+      </c>
+      <c r="P9" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C10">
-        <v>1045</v>
+        <v>1280</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2770,24 +3162,30 @@
         <v>0</v>
       </c>
       <c r="J10" s="3">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="K10" s="3">
-        <v>1.95</v>
+        <v>1.45</v>
       </c>
       <c r="L10">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="M10" s="5">
-        <v>9.3000000000000007</v>
+        <v>6.45</v>
+      </c>
+      <c r="P10" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>105</v>
       </c>
       <c r="C11">
-        <v>847</v>
+        <v>1045</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2808,24 +3206,27 @@
         <v>0</v>
       </c>
       <c r="J11" s="3">
-        <v>5.18</v>
+        <v>4.2</v>
       </c>
       <c r="K11" s="3">
-        <v>1.01</v>
+        <v>1.95</v>
       </c>
       <c r="L11">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="M11" s="5">
-        <v>10</v>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="P11" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="C12">
-        <v>570</v>
+        <v>847</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2846,30 +3247,33 @@
         <v>0</v>
       </c>
       <c r="J12" s="3">
-        <v>4.3600000000000003</v>
+        <v>5.18</v>
       </c>
       <c r="K12" s="3">
-        <v>2.25</v>
+        <v>1.01</v>
+      </c>
+      <c r="L12">
+        <v>50</v>
       </c>
       <c r="M12" s="5">
-        <v>8.25</v>
+        <v>10</v>
+      </c>
+      <c r="P12" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="C13">
-        <v>1070</v>
+        <v>570</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -2884,30 +3288,33 @@
         <v>0</v>
       </c>
       <c r="J13" s="3">
-        <v>4.57</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="K13" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="L13">
-        <v>107</v>
+        <v>2.25</v>
       </c>
       <c r="M13" s="5">
-        <v>11</v>
+        <v>8.25</v>
+      </c>
+      <c r="P13" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
       </c>
       <c r="C14">
-        <v>1160</v>
+        <v>1070</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -2922,27 +3329,27 @@
         <v>0</v>
       </c>
       <c r="J14" s="3">
-        <v>3.68</v>
+        <v>4.57</v>
       </c>
       <c r="K14" s="3">
-        <v>1.38</v>
+        <v>1.3</v>
       </c>
       <c r="L14">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="M14" s="5">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="P14" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C15">
-        <v>837</v>
+        <v>1160</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2957,33 +3364,36 @@
         <v>0</v>
       </c>
       <c r="H15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="3">
-        <v>4.55</v>
+        <v>3.68</v>
       </c>
       <c r="K15" s="3">
-        <v>2.35</v>
+        <v>1.38</v>
       </c>
       <c r="L15">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M15" s="5">
-        <v>11.8</v>
-      </c>
-      <c r="N15" s="5">
-        <v>15.5</v>
+        <v>7</v>
+      </c>
+      <c r="P15" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
       </c>
       <c r="C16">
-        <v>1100</v>
+        <v>837</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2998,33 +3408,36 @@
         <v>0</v>
       </c>
       <c r="H16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="3">
-        <v>4</v>
+        <v>4.55</v>
       </c>
       <c r="K16" s="3">
-        <v>1.42</v>
+        <v>2.35</v>
       </c>
       <c r="L16">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="M16" s="5">
-        <v>8.9499999999999993</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>11.8</v>
+      </c>
+      <c r="N16" s="5">
+        <v>15.5</v>
+      </c>
+      <c r="P16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C17">
-        <v>1628</v>
+        <v>1100</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -3045,27 +3458,30 @@
         <v>0</v>
       </c>
       <c r="J17" s="3">
-        <v>2.36</v>
+        <v>4</v>
       </c>
       <c r="K17" s="3">
-        <v>1.1200000000000001</v>
+        <v>1.42</v>
       </c>
       <c r="L17">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="M17" s="5">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="P17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C18">
-        <v>1000</v>
+        <v>1628</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -3086,24 +3502,30 @@
         <v>0</v>
       </c>
       <c r="J18" s="3">
-        <v>4.42</v>
+        <v>2.36</v>
       </c>
       <c r="K18" s="3">
-        <v>1.64</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="L18">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="M18" s="5">
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.3</v>
+      </c>
+      <c r="P18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
       </c>
       <c r="C19">
-        <v>1142</v>
+        <v>1000</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -3124,24 +3546,27 @@
         <v>0</v>
       </c>
       <c r="J19" s="3">
-        <v>3.78</v>
+        <v>4.42</v>
       </c>
       <c r="K19" s="3">
-        <v>1.55</v>
+        <v>1.64</v>
       </c>
       <c r="L19">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="M19" s="5">
-        <v>8.36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="P19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20">
-        <v>1105</v>
+        <v>1142</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -3162,27 +3587,27 @@
         <v>0</v>
       </c>
       <c r="J20" s="3">
-        <v>3.9</v>
+        <v>3.78</v>
       </c>
       <c r="K20" s="3">
-        <v>1.75</v>
+        <v>1.55</v>
       </c>
       <c r="L20">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="M20" s="5">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>8.36</v>
+      </c>
+      <c r="P20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="C21">
-        <v>1124</v>
+        <v>1105</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -3203,27 +3628,30 @@
         <v>0</v>
       </c>
       <c r="J21" s="3">
-        <v>3.88</v>
+        <v>3.9</v>
       </c>
       <c r="K21" s="3">
-        <v>1.37</v>
+        <v>1.75</v>
       </c>
       <c r="L21">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="M21" s="5">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+      <c r="P21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
         <v>104</v>
       </c>
       <c r="C22">
-        <v>1075</v>
+        <v>1124</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -3244,27 +3672,30 @@
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <v>4.3899999999999997</v>
+        <v>3.88</v>
       </c>
       <c r="K22" s="3">
-        <v>1.5</v>
+        <v>1.37</v>
       </c>
       <c r="L22">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M22" s="5">
-        <v>8.2200000000000006</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6.5</v>
+      </c>
+      <c r="P22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C23">
-        <v>1400</v>
+        <v>1075</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3285,27 +3716,30 @@
         <v>0</v>
       </c>
       <c r="J23" s="3">
-        <v>3.4</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="K23" s="3">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="L23">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="M23" s="5">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="P23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
         <v>107</v>
       </c>
       <c r="C24">
-        <v>1347</v>
+        <v>1400</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -3335,18 +3769,21 @@
         <v>45</v>
       </c>
       <c r="M24" s="5">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>4.2</v>
+      </c>
+      <c r="P24" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
         <v>107</v>
       </c>
       <c r="C25">
-        <v>1294</v>
+        <v>1347</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -3376,15 +3813,21 @@
         <v>45</v>
       </c>
       <c r="M25" s="5">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>5.3</v>
+      </c>
+      <c r="P25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>109</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
       </c>
       <c r="C26">
-        <v>570</v>
+        <v>1294</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -3405,21 +3848,65 @@
         <v>0</v>
       </c>
       <c r="J26" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="K26" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="L26">
+        <v>45</v>
+      </c>
+      <c r="M26" s="5">
+        <v>6.4</v>
+      </c>
+      <c r="P26" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27">
+        <v>570</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27" s="3">
         <v>3.35</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K27" s="3">
         <v>2.25</v>
       </c>
-      <c r="L26">
+      <c r="L27">
         <v>48</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M27" s="5">
         <v>8.1999999999999993</v>
       </c>
+      <c r="P27" t="s">
+        <v>195</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P26">
-    <sortCondition ref="A2:A26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P27">
+    <sortCondition ref="A2:A27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3429,22 +3916,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8313B353-BF25-43AE-B003-13E2A48F1E77}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="3"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="0" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="5" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="5" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3540,6 +4028,9 @@
       <c r="O2" t="s">
         <v>125</v>
       </c>
+      <c r="P2" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -3582,7 +4073,7 @@
         <v>126</v>
       </c>
       <c r="P3" t="s">
-        <v>128</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -3631,6 +4122,9 @@
       <c r="O4" t="s">
         <v>127</v>
       </c>
+      <c r="P4" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -3675,6 +4169,9 @@
       <c r="N5" s="5">
         <v>16.829999999999998</v>
       </c>
+      <c r="P5" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3716,6 +4213,9 @@
       <c r="N6" s="5">
         <v>38</v>
       </c>
+      <c r="P6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3757,6 +4257,9 @@
       <c r="N7" s="5">
         <v>25.1</v>
       </c>
+      <c r="P7" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -3798,6 +4301,9 @@
       <c r="M8" s="5">
         <v>11.61</v>
       </c>
+      <c r="P8" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -3839,6 +4345,9 @@
       <c r="N9" s="5">
         <v>16.8</v>
       </c>
+      <c r="P9" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3880,6 +4389,9 @@
       <c r="N10" s="5">
         <v>29.2</v>
       </c>
+      <c r="P10" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -3924,6 +4436,9 @@
       <c r="N11" s="5">
         <v>17.399999999999999</v>
       </c>
+      <c r="P11" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -3965,6 +4480,9 @@
       <c r="N12" s="5">
         <v>4.25</v>
       </c>
+      <c r="P12" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -4003,6 +4521,9 @@
       <c r="N13" s="5">
         <v>21</v>
       </c>
+      <c r="P13" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -4044,6 +4565,9 @@
       <c r="N14" s="5">
         <v>9.2799999999999994</v>
       </c>
+      <c r="P14" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -4082,6 +4606,9 @@
       <c r="M15" s="5">
         <v>10.7</v>
       </c>
+      <c r="P15" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -4123,8 +4650,11 @@
       <c r="N16" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4164,8 +4694,11 @@
       <c r="M17" s="5">
         <v>8.36</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -4208,8 +4741,11 @@
       <c r="N18" s="5">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -4249,8 +4785,11 @@
       <c r="N19" s="5">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -4287,8 +4826,11 @@
       <c r="M20" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -4325,8 +4867,11 @@
       <c r="M21" s="5">
         <v>9.75</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -4366,8 +4911,11 @@
       <c r="N22" s="5">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -4407,8 +4955,11 @@
       <c r="N23" s="5">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -4448,8 +4999,11 @@
       <c r="N24" s="5">
         <v>11.15</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -4489,8 +5043,11 @@
       <c r="N25" s="5">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P25" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -4530,8 +5087,11 @@
       <c r="N26" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -4571,8 +5131,11 @@
       <c r="N27" s="5">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -4612,8 +5175,11 @@
       <c r="N28" s="5">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P28" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -4650,8 +5216,11 @@
       <c r="M29" s="5">
         <v>8.6</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P29" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -4691,8 +5260,11 @@
       <c r="N30" s="5">
         <v>17.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P30" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>89</v>
       </c>
@@ -4732,8 +5304,11 @@
       <c r="N31" s="5">
         <v>11.14</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P31" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -4776,8 +5351,11 @@
       <c r="N32" s="5">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>91</v>
       </c>
@@ -4814,8 +5392,11 @@
       <c r="M33" s="5">
         <v>11.8</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P33" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -4855,8 +5436,11 @@
       <c r="N34" s="5">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P34" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -4895,6 +5479,9 @@
       </c>
       <c r="N35" s="5">
         <v>13.5</v>
+      </c>
+      <c r="P35" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -4910,7 +5497,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4924,7 +5511,7 @@
     <col min="13" max="13" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5014,6 +5601,9 @@
       <c r="M2" s="5">
         <v>8.0399999999999991</v>
       </c>
+      <c r="P2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5052,6 +5642,9 @@
       <c r="M3" s="5">
         <v>12.29</v>
       </c>
+      <c r="P3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -5090,6 +5683,9 @@
       <c r="M4" s="5">
         <v>16.079999999999998</v>
       </c>
+      <c r="P4" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -5131,6 +5727,9 @@
       <c r="N5" s="5">
         <v>21</v>
       </c>
+      <c r="P5" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -5172,6 +5771,9 @@
       <c r="N6" s="5">
         <v>15.91</v>
       </c>
+      <c r="P6" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -5213,6 +5815,9 @@
       <c r="N7" s="5">
         <v>17.829999999999998</v>
       </c>
+      <c r="P7" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -5254,6 +5859,9 @@
       <c r="N8" s="5">
         <v>16.5</v>
       </c>
+      <c r="P8" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -5295,6 +5903,9 @@
       <c r="N9" s="5">
         <v>21</v>
       </c>
+      <c r="P9" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -5336,6 +5947,9 @@
       <c r="N10" s="5">
         <v>17.5</v>
       </c>
+      <c r="P10" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -5377,6 +5991,9 @@
       <c r="N11" s="5">
         <v>21</v>
       </c>
+      <c r="P11" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -5418,6 +6035,9 @@
       <c r="N12" s="5">
         <v>27.66</v>
       </c>
+      <c r="P12" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -5458,6 +6078,9 @@
       </c>
       <c r="N13" s="5">
         <v>18</v>
+      </c>
+      <c r="P13" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated logo paths in db
</commit_message>
<xml_diff>
--- a/dinghies.xlsx
+++ b/dinghies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\iain\Development\dinghy-search\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soarsi\workspace\github\dinghy-search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B009F385-DD3F-49ED-90E5-5EB0990D3884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B0DA13-D78C-480A-83AA-D79E8F01CC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="948" windowWidth="14340" windowHeight="8880" xr2:uid="{424A2331-99F2-4D2E-BF59-9192B1CDA9D6}"/>
+    <workbookView xWindow="-27300" yWindow="2025" windowWidth="25365" windowHeight="13170" xr2:uid="{424A2331-99F2-4D2E-BF59-9192B1CDA9D6}"/>
   </bookViews>
   <sheets>
     <sheet name="RS" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="314">
   <si>
     <t>name</t>
   </si>
@@ -441,42 +441,9 @@
     <t>/images/logos/RS800.png</t>
   </si>
   <si>
-    <t>/images/logos/RS-Feva-logo.jpg</t>
-  </si>
-  <si>
-    <t>/images/logos/RS-neo-horizontal.png</t>
-  </si>
-  <si>
-    <t>/images/logos/RSQuest.png</t>
-  </si>
-  <si>
-    <t>/images/logos/RSVenture.png</t>
-  </si>
-  <si>
-    <t>/images/logos/RSTera.png</t>
-  </si>
-  <si>
-    <t>/images/logos/Toura-Master-300x171.png</t>
-  </si>
-  <si>
-    <t>/images/logos/RSVareo-logo.png</t>
-  </si>
-  <si>
-    <t>/images/logos/Logo-RS-Zest.png</t>
-  </si>
-  <si>
     <t>/images/logos/RS100.png</t>
   </si>
   <si>
-    <t>/images/logos/RS400-magenta.png</t>
-  </si>
-  <si>
-    <t>/images/logos/RS600_Logo_New_Black-300x114.png</t>
-  </si>
-  <si>
-    <t>/images/logos/RSVision.jpg</t>
-  </si>
-  <si>
     <t>/images/aero-5.jpg</t>
   </si>
   <si>
@@ -970,6 +937,51 @@
   </si>
   <si>
     <t>/images/logos/rs-cat16.png</t>
+  </si>
+  <si>
+    <t>/images/logos/49er-49erfx.png</t>
+  </si>
+  <si>
+    <t>/images/logos/enterprise.png</t>
+  </si>
+  <si>
+    <t>/images/logos/firefly.png</t>
+  </si>
+  <si>
+    <t>/images/logos/comet-trio.png</t>
+  </si>
+  <si>
+    <t>/images/logos/rs-feva.jpg</t>
+  </si>
+  <si>
+    <t>/images/logos/rs-neo.png</t>
+  </si>
+  <si>
+    <t>/images/logos/rs-quest.png</t>
+  </si>
+  <si>
+    <t>/images/logos/rs-tera.png</t>
+  </si>
+  <si>
+    <t>/images/logos/rs-toura.png</t>
+  </si>
+  <si>
+    <t>/images/logos/rs-vareo.png</t>
+  </si>
+  <si>
+    <t>/images/logos/rs-venture.png</t>
+  </si>
+  <si>
+    <t>/images/logos/rs-vision.jpg</t>
+  </si>
+  <si>
+    <t>/images/logos/rs-zest.png</t>
+  </si>
+  <si>
+    <t>/images/logos/RS400.png</t>
+  </si>
+  <si>
+    <t>/images/logos/RS600.png</t>
   </si>
 </sst>
 </file>
@@ -1360,27 +1372,27 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="3" customWidth="1"/>
     <col min="11" max="11" width="6" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="5" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1430,7 +1442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2000</v>
       </c>
@@ -1474,10 +1486,10 @@
         <v>127</v>
       </c>
       <c r="P2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1518,13 +1530,13 @@
         <v>5.2</v>
       </c>
       <c r="O3" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="P3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1565,13 +1577,13 @@
         <v>6.3</v>
       </c>
       <c r="O4" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="P4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1612,13 +1624,13 @@
         <v>7.4</v>
       </c>
       <c r="O5" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="P5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1659,13 +1671,13 @@
         <v>8.9</v>
       </c>
       <c r="O6" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="P6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1706,13 +1718,13 @@
         <v>9</v>
       </c>
       <c r="O7" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="P7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1753,13 +1765,13 @@
         <v>12.82</v>
       </c>
       <c r="O8" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="P8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1803,13 +1815,13 @@
         <v>7</v>
       </c>
       <c r="O9" t="s">
-        <v>133</v>
+        <v>303</v>
       </c>
       <c r="P9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1847,13 +1859,13 @@
         <v>6</v>
       </c>
       <c r="O10" t="s">
-        <v>134</v>
+        <v>304</v>
       </c>
       <c r="P10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1894,13 +1906,13 @@
         <v>11</v>
       </c>
       <c r="O11" t="s">
-        <v>135</v>
+        <v>305</v>
       </c>
       <c r="P11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1941,13 +1953,13 @@
         <v>4.8</v>
       </c>
       <c r="O12" t="s">
-        <v>137</v>
+        <v>306</v>
       </c>
       <c r="P12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1988,13 +2000,13 @@
         <v>3.7</v>
       </c>
       <c r="O13" t="s">
-        <v>137</v>
+        <v>306</v>
       </c>
       <c r="P13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2035,13 +2047,13 @@
         <v>14.6</v>
       </c>
       <c r="O14" t="s">
-        <v>138</v>
+        <v>307</v>
       </c>
       <c r="P14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2085,13 +2097,13 @@
         <v>9.9</v>
       </c>
       <c r="O15" t="s">
-        <v>139</v>
+        <v>308</v>
       </c>
       <c r="P15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2132,13 +2144,13 @@
         <v>14</v>
       </c>
       <c r="O16" t="s">
-        <v>136</v>
+        <v>309</v>
       </c>
       <c r="P16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2182,13 +2194,13 @@
         <v>12</v>
       </c>
       <c r="O17" t="s">
+        <v>310</v>
+      </c>
+      <c r="P17" t="s">
         <v>144</v>
       </c>
-      <c r="P17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2226,13 +2238,13 @@
         <v>7.1</v>
       </c>
       <c r="O18" t="s">
-        <v>140</v>
+        <v>311</v>
       </c>
       <c r="P18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2273,13 +2285,13 @@
         <v>12.5</v>
       </c>
       <c r="O19" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="P19" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2323,13 +2335,13 @@
         <v>12.5</v>
       </c>
       <c r="O20" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="P20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2376,10 +2388,10 @@
         <v>128</v>
       </c>
       <c r="P21" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2423,10 +2435,10 @@
         <v>129</v>
       </c>
       <c r="P22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2470,13 +2482,13 @@
         <v>13.94</v>
       </c>
       <c r="O23" t="s">
-        <v>142</v>
+        <v>312</v>
       </c>
       <c r="P23" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -2523,10 +2535,10 @@
         <v>130</v>
       </c>
       <c r="P24" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2567,13 +2579,13 @@
         <v>12.14</v>
       </c>
       <c r="O25" t="s">
-        <v>143</v>
+        <v>313</v>
       </c>
       <c r="P25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2620,10 +2632,10 @@
         <v>131</v>
       </c>
       <c r="P26" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2670,7 +2682,7 @@
         <v>132</v>
       </c>
       <c r="P27" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2690,16 +2702,16 @@
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.109375" style="3"/>
-    <col min="13" max="13" width="9.109375" style="5"/>
-    <col min="15" max="15" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="3"/>
+    <col min="13" max="13" width="9.140625" style="5"/>
+    <col min="15" max="15" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2749,7 +2761,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -2793,10 +2805,10 @@
         <v>124</v>
       </c>
       <c r="P2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -2840,10 +2852,10 @@
         <v>124</v>
       </c>
       <c r="P3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -2887,7 +2899,7 @@
         <v>124</v>
       </c>
       <c r="P4" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2904,24 +2916,24 @@
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="5" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="32.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="11" width="8.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2971,7 +2983,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -3012,13 +3024,13 @@
         <v>10.4</v>
       </c>
       <c r="O2" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="P2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -3059,15 +3071,15 @@
         <v>6.8</v>
       </c>
       <c r="O3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="P3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="C4">
         <v>1210</v>
@@ -3103,13 +3115,13 @@
         <v>6.5</v>
       </c>
       <c r="O4" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="P4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -3150,13 +3162,13 @@
         <v>10.3</v>
       </c>
       <c r="O5" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="P5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -3200,13 +3212,13 @@
         <v>13.2</v>
       </c>
       <c r="O6" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="P6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -3247,13 +3259,13 @@
         <v>8.1</v>
       </c>
       <c r="O7" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="P7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -3291,13 +3303,13 @@
         <v>7</v>
       </c>
       <c r="O8" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="P8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -3338,13 +3350,13 @@
         <v>10</v>
       </c>
       <c r="O9" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="P9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -3385,13 +3397,13 @@
         <v>6.45</v>
       </c>
       <c r="O10" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="P10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -3432,13 +3444,13 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="O11" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="P11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -3476,13 +3488,13 @@
         <v>10</v>
       </c>
       <c r="O12" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="P12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -3517,13 +3529,13 @@
         <v>8.25</v>
       </c>
       <c r="O13" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="P13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -3564,13 +3576,13 @@
         <v>11</v>
       </c>
       <c r="O14" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="P14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -3608,13 +3620,13 @@
         <v>7</v>
       </c>
       <c r="O15" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="P15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -3658,13 +3670,13 @@
         <v>15.5</v>
       </c>
       <c r="O16" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="P16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -3702,13 +3714,13 @@
         <v>8.9499999999999993</v>
       </c>
       <c r="O17" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="P17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -3749,13 +3761,13 @@
         <v>3.3</v>
       </c>
       <c r="O18" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="P18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3796,13 +3808,13 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="O19" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="P19" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -3840,13 +3852,13 @@
         <v>8.36</v>
       </c>
       <c r="O20" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="P20" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -3884,13 +3896,13 @@
         <v>8.5</v>
       </c>
       <c r="O21" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="P21" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -3931,13 +3943,13 @@
         <v>6.5</v>
       </c>
       <c r="O22" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="P22" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -3978,13 +3990,13 @@
         <v>8.2200000000000006</v>
       </c>
       <c r="O23" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="P23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -4025,13 +4037,13 @@
         <v>4.2</v>
       </c>
       <c r="O24" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="P24" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -4072,13 +4084,13 @@
         <v>5.3</v>
       </c>
       <c r="O25" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="P25" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -4119,13 +4131,13 @@
         <v>6.4</v>
       </c>
       <c r="O26" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="P26" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -4163,10 +4175,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="O27" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="P27" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -4181,26 +4193,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8313B353-BF25-43AE-B003-13E2A48F1E77}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="5" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="11" width="8.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4250,7 +4262,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>420</v>
       </c>
@@ -4291,13 +4303,13 @@
         <v>9</v>
       </c>
       <c r="O2" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="P2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>470</v>
       </c>
@@ -4335,13 +4347,13 @@
         <v>13</v>
       </c>
       <c r="O3" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="P3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>505</v>
       </c>
@@ -4385,13 +4397,13 @@
         <v>26</v>
       </c>
       <c r="O4" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="P4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -4435,13 +4447,13 @@
         <v>16.829999999999998</v>
       </c>
       <c r="O5" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="P5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -4481,11 +4493,14 @@
       <c r="N6" s="5">
         <v>38</v>
       </c>
+      <c r="O6" t="s">
+        <v>299</v>
+      </c>
       <c r="P6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -4525,11 +4540,14 @@
       <c r="N7" s="5">
         <v>25.1</v>
       </c>
+      <c r="O7" t="s">
+        <v>299</v>
+      </c>
       <c r="P7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -4570,13 +4588,13 @@
         <v>11.61</v>
       </c>
       <c r="O8" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="P8" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -4617,13 +4635,13 @@
         <v>16.8</v>
       </c>
       <c r="O9" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="P9" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -4664,13 +4682,13 @@
         <v>29.2</v>
       </c>
       <c r="O10" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="P10" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -4714,13 +4732,13 @@
         <v>17.399999999999999</v>
       </c>
       <c r="O11" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="P11" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -4761,13 +4779,13 @@
         <v>4.25</v>
       </c>
       <c r="O12" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="P12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>114</v>
       </c>
@@ -4805,13 +4823,13 @@
         <v>21</v>
       </c>
       <c r="O13" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="P13" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -4851,11 +4869,14 @@
       <c r="N14" s="5">
         <v>9.2799999999999994</v>
       </c>
+      <c r="O14" t="s">
+        <v>302</v>
+      </c>
       <c r="P14" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -4892,11 +4913,14 @@
       <c r="M15" s="5">
         <v>10.7</v>
       </c>
+      <c r="O15" t="s">
+        <v>300</v>
+      </c>
       <c r="P15" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -4937,13 +4961,13 @@
         <v>13</v>
       </c>
       <c r="O16" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="P16" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4983,11 +5007,14 @@
       <c r="M17" s="5">
         <v>8.36</v>
       </c>
+      <c r="O17" t="s">
+        <v>301</v>
+      </c>
       <c r="P17" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -5031,13 +5058,13 @@
         <v>14.2</v>
       </c>
       <c r="O18" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="P18" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -5078,13 +5105,13 @@
         <v>8.4</v>
       </c>
       <c r="O19" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="P19" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -5122,13 +5149,13 @@
         <v>10</v>
       </c>
       <c r="O20" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="P20" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -5166,13 +5193,13 @@
         <v>9.75</v>
       </c>
       <c r="O21" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="P21" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -5213,13 +5240,13 @@
         <v>32</v>
       </c>
       <c r="O22" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="P22" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -5260,13 +5287,13 @@
         <v>29</v>
       </c>
       <c r="O23" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="P23" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -5307,13 +5334,13 @@
         <v>11.15</v>
       </c>
       <c r="O24" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="P24" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -5354,13 +5381,13 @@
         <v>7.4</v>
       </c>
       <c r="O25" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="P25" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -5401,13 +5428,13 @@
         <v>10</v>
       </c>
       <c r="O26" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="P26" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -5448,13 +5475,13 @@
         <v>7.4</v>
       </c>
       <c r="O27" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="P27" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -5495,13 +5522,13 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="O28" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="P28" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -5539,13 +5566,13 @@
         <v>8.6</v>
       </c>
       <c r="O29" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="P29" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -5589,13 +5616,13 @@
         <v>17.2</v>
       </c>
       <c r="O30" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="P30" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>89</v>
       </c>
@@ -5636,13 +5663,13 @@
         <v>11.14</v>
       </c>
       <c r="O31" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="P31" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -5686,13 +5713,13 @@
         <v>12.5</v>
       </c>
       <c r="O32" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="P32" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>91</v>
       </c>
@@ -5730,13 +5757,13 @@
         <v>11.8</v>
       </c>
       <c r="O33" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="P33" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -5777,13 +5804,13 @@
         <v>9.9</v>
       </c>
       <c r="O34" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="P34" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -5824,10 +5851,10 @@
         <v>13.5</v>
       </c>
       <c r="O35" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="P35" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -5846,23 +5873,23 @@
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="11" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5912,7 +5939,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -5950,13 +5977,13 @@
         <v>8.0399999999999991</v>
       </c>
       <c r="O2" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="P2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -5994,13 +6021,13 @@
         <v>12.29</v>
       </c>
       <c r="O3" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="P3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -6038,13 +6065,13 @@
         <v>16.079999999999998</v>
       </c>
       <c r="O4" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="P4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -6085,13 +6112,13 @@
         <v>21</v>
       </c>
       <c r="O5" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="P5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -6132,13 +6159,13 @@
         <v>15.91</v>
       </c>
       <c r="O6" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="P6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>122</v>
       </c>
@@ -6179,13 +6206,13 @@
         <v>17.829999999999998</v>
       </c>
       <c r="O7" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="P7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -6226,13 +6253,13 @@
         <v>16.5</v>
       </c>
       <c r="O8" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="P8" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -6273,13 +6300,13 @@
         <v>21</v>
       </c>
       <c r="O9" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="P9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>119</v>
       </c>
@@ -6320,13 +6347,13 @@
         <v>17.5</v>
       </c>
       <c r="O10" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="P10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>120</v>
       </c>
@@ -6367,13 +6394,13 @@
         <v>21</v>
       </c>
       <c r="O11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="P11" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>121</v>
       </c>
@@ -6414,13 +6441,13 @@
         <v>27.66</v>
       </c>
       <c r="O12" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="P12" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -6461,10 +6488,10 @@
         <v>18</v>
       </c>
       <c r="O13" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="P13" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>